<commit_message>
Switches excel file correction
</commit_message>
<xml_diff>
--- a/switches.xlsx
+++ b/switches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Abhinay\Python\Port Status\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Abhinay\Python\Git - Network Automation\network_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269DA946-94A0-4D31-BBD0-7140DF82EC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9FFED0-CE52-4892-B0FC-FC9F2021E0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,48 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>usrosd400bsw03</t>
-  </si>
-  <si>
-    <t>10.0.44.60</t>
-  </si>
-  <si>
-    <t>usrosd405-pclab01</t>
-  </si>
-  <si>
-    <t>10.0.44.35</t>
-  </si>
-  <si>
-    <t>usrosd405-pclab02</t>
-  </si>
-  <si>
-    <t>10.0.44.244</t>
-  </si>
-  <si>
-    <t>usrosd451sw01</t>
-  </si>
-  <si>
-    <t>10.0.44.62</t>
-  </si>
-  <si>
-    <t>usrosd455_labsw01</t>
-  </si>
-  <si>
-    <t>10.0.44.144</t>
-  </si>
-  <si>
-    <t>usrosd530bsw01</t>
-  </si>
-  <si>
-    <t>10.0.44.32</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>hostname</t>
   </si>
   <si>
     <t>ip</t>
+  </si>
+  <si>
+    <t>&lt;Enter Hostname&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Enter Device IP&gt;</t>
   </si>
 </sst>
 </file>
@@ -404,71 +374,51 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>